<commit_message>
added function for observations scaling, prepared repo for using with colab later.
</commit_message>
<xml_diff>
--- a/old/data and code structure.xlsx
+++ b/old/data and code structure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\PycharmProjects\finrlpaper2\MT-DRL-Pytorch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\PycharmProjects\finrlpaper2\MT-DRL-Pytorch\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80842BE-7085-4628-A348-D3FBBD226A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B414F43-8C8C-4802-B4D9-9CB33AD6E73C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19298" yWindow="420" windowWidth="19396" windowHeight="10395" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithms" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="300">
   <si>
     <t>stable_baselines3</t>
   </si>
@@ -923,13 +923,19 @@
   </si>
   <si>
     <t>The output policy is a probability distribution over actions (e.g. gaussian?) ?</t>
+  </si>
+  <si>
+    <t>dropped</t>
+  </si>
+  <si>
+    <t>&lt;= final composition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -954,6 +960,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1015,7 +1028,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1031,6 +1044,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1688,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B8548A-43D0-4877-A3FC-D8C353B86AF4}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,8 +1794,11 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="11" t="s">
         <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>298</v>
       </c>
       <c r="G7" t="s">
         <v>117</v>
@@ -1834,8 +1853,11 @@
       <c r="A11" t="s">
         <v>73</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="12" t="s">
         <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>298</v>
       </c>
       <c r="G11" t="s">
         <v>106</v>
@@ -1943,8 +1965,11 @@
       <c r="A19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="12" t="s">
         <v>80</v>
+      </c>
+      <c r="C19" t="s">
+        <v>298</v>
       </c>
       <c r="G19" t="s">
         <v>126</v>
@@ -2013,8 +2038,11 @@
       <c r="A24" t="s">
         <v>85</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="12" t="s">
         <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>298</v>
       </c>
       <c r="G24" t="s">
         <v>110</v>
@@ -2069,8 +2097,11 @@
       <c r="A28" t="s">
         <v>89</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="12" t="s">
         <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>298</v>
       </c>
       <c r="G28" t="s">
         <v>111</v>
@@ -2111,8 +2142,11 @@
       <c r="A31" t="s">
         <v>92</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="12" t="s">
         <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>298</v>
       </c>
       <c r="G31" t="s">
         <v>134</v>
@@ -2174,6 +2208,15 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>299</v>
+      </c>
       <c r="G37" t="s">
         <v>114</v>
       </c>
@@ -2182,59 +2225,248 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="N38" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="N39" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="N40" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="N41" t="s">
         <v>146</v>
       </c>
     </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="N43" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="N44" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="N45" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="N46" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="N47" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>13</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="N49" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>14</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="N50" t="s">
         <v>149</v>
       </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>17</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>18</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>19</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>20</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>21</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>22</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>23</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>24</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>25</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>26</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>27</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2767,8 +2999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1DFCA7-A683-4EEC-8AFF-B461F35029B5}">
   <dimension ref="B5:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>